<commit_message>
[bugs] added shared_strings capability and string to number conversion in read_cells() + tests
</commit_message>
<xml_diff>
--- a/example/example2.xlsx
+++ b/example/example2.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Shared_formula" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,8 +19,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>more text</t>
+  </si>
+  <si>
+    <t>again more tewt</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>erz</t>
+  </si>
+  <si>
+    <t>ezr</t>
+  </si>
+  <si>
+    <t>zaeze</t>
+  </si>
+  <si>
+    <t>Romain</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -49,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -431,7 +465,7 @@
         <f t="shared" ref="B2:B4" si="0">A2 * 2</f>
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>D1 + 10 * I1 + $A$1</f>
         <v>22</v>
       </c>
@@ -450,11 +484,11 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>3</v>
+        <v>3.2323</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>6.4645999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -464,6 +498,91 @@
       <c r="B4">
         <f t="shared" si="0"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:G17" si="2">A1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>3.2323</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7">
+      <c r="G18">
+        <f>A4</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[bug] fixed pb with unicode and shared strings + adapted test
</commit_message>
<xml_diff>
--- a/example/example2.xlsx
+++ b/example/example2.xlsx
@@ -50,9 +50,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -84,7 +81,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +416,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -548,13 +545,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="7:7">
+    <row r="17" spans="2:7">
       <c r="G17">
         <f t="shared" si="2"/>
         <v>3.2323</v>
       </c>
     </row>
-    <row r="18" spans="7:7">
+    <row r="18" spans="2:7">
+      <c r="B18" t="str">
+        <f>B12</f>
+        <v>again more tewt</v>
+      </c>
       <c r="G18">
         <f>A4</f>
         <v>4</v>

</xml_diff>